<commit_message>
Fix living wiht mother
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_VISIT/forms/CRIANCA_VISIT/CRIANCA_VISIT.xlsx
+++ b/app/config/tables/CRIANCA_VISIT/forms/CRIANCA_VISIT/CRIANCA_VISIT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E3F5B2-776A-4EB4-BB3F-C8E98F6DB0E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459BB7CB-304C-49BF-9F84-74416EB7322B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -609,9 +609,6 @@
     <t>Age of stopping breastfeeding</t>
   </si>
   <si>
-    <t>data('moma') != '1'</t>
-  </si>
-  <si>
     <t>DASEP</t>
   </si>
   <si>
@@ -673,6 +670,9 @@
   </si>
   <si>
     <t>Nunca</t>
+  </si>
+  <si>
+    <t>data('moma') != '2'</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1164,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1218,9 +1218,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1374,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
@@ -1570,7 +1570,7 @@
         <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
         <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1656,7 +1656,7 @@
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -1713,7 +1713,7 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1732,10 +1732,10 @@
         <v>138</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1743,7 +1743,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1751,13 +1751,13 @@
         <v>31</v>
       </c>
       <c r="F53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1765,13 +1765,13 @@
         <v>170</v>
       </c>
       <c r="F54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1779,13 +1779,13 @@
         <v>60</v>
       </c>
       <c r="F55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1952,7 +1952,7 @@
         <v>51</v>
       </c>
       <c r="C76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
         <v>51</v>
       </c>
       <c r="C90" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -2181,10 +2181,10 @@
         <v>175</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s">
         <v>177</v>
@@ -2268,7 +2268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
@@ -2553,10 +2553,10 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" t="s">
         <v>212</v>
-      </c>
-      <c r="D19" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
         <v>170</v>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B26" t="s">
         <v>170</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
Bednet, BSG og Vac Card ændringer
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_VISIT/forms/CRIANCA_VISIT/CRIANCA_VISIT.xlsx
+++ b/app/config/tables/CRIANCA_VISIT/forms/CRIANCA_VISIT/CRIANCA_VISIT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60014AB1-3F9A-4308-949D-F55E2DFBCA1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4158F7-B625-48B5-95BF-9CD5731DC22E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="215">
   <si>
     <t>setting_name</t>
   </si>
@@ -267,60 +267,15 @@
     <t>VIC</t>
   </si>
   <si>
-    <t>Card seen</t>
-  </si>
-  <si>
-    <t>Cartão visto</t>
-  </si>
-  <si>
     <t>NTN</t>
   </si>
   <si>
-    <t>Has no card and no vaccines</t>
-  </si>
-  <si>
-    <t>Não tem cartão e não tem vacinas</t>
-  </si>
-  <si>
     <t>NTS</t>
   </si>
   <si>
-    <t>Has no card, some vaccines</t>
-  </si>
-  <si>
-    <t>Não tem cartão, mas tem vacinas</t>
-  </si>
-  <si>
-    <t>NVC</t>
-  </si>
-  <si>
-    <t>Not brought card</t>
-  </si>
-  <si>
-    <t>Não trouxe o cartão</t>
-  </si>
-  <si>
     <t>PC</t>
   </si>
   <si>
-    <t>Lost card</t>
-  </si>
-  <si>
-    <t>Perdeu o cartão</t>
-  </si>
-  <si>
-    <t>VCN</t>
-  </si>
-  <si>
-    <t>Card seen and NO vaccines</t>
-  </si>
-  <si>
-    <t>Cartão visto, mas sem vacinas registadas</t>
-  </si>
-  <si>
-    <t>Vaccination cart</t>
-  </si>
-  <si>
     <t>Cartão de vacina</t>
   </si>
   <si>
@@ -345,9 +300,6 @@
     <t>Todo tempo?</t>
   </si>
   <si>
-    <t>data('TENDAYN') == '1'</t>
-  </si>
-  <si>
     <t>bednet</t>
   </si>
   <si>
@@ -685,6 +637,45 @@
   </si>
   <si>
     <t>{REGIDC: data('REGIDC'), VISITDATE: data('CONT'), VISITIDC: opendatakit.getCurrentInstanceId()}</t>
+  </si>
+  <si>
+    <t>data('TENDAYN') != '2' || data('TENDA') !=3</t>
+  </si>
+  <si>
+    <t>Scar</t>
+  </si>
+  <si>
+    <t>Yes but it is changing</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Sim, mas change</t>
+  </si>
+  <si>
+    <t>Cartão visto (S.V)</t>
+  </si>
+  <si>
+    <t>Card seen (S.V)</t>
+  </si>
+  <si>
+    <t>Does the child have a vaccination cart</t>
+  </si>
+  <si>
+    <t>Dosn't have a card (NT)</t>
+  </si>
+  <si>
+    <t>Não tem cartão (NT)</t>
+  </si>
+  <si>
+    <t>Has card, but i has not been seen (NVC)</t>
+  </si>
+  <si>
+    <t>Lost card (CP)</t>
+  </si>
+  <si>
+    <t>Perdeu o cartão (CP)</t>
   </si>
 </sst>
 </file>
@@ -1155,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1179,10 +1170,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1234,8 +1225,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1289,7 @@
         <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
         <v>49</v>
@@ -1312,7 +1303,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1351,7 +1342,7 @@
         <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,23 +1361,23 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="17" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1400,7 +1391,7 @@
         <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1414,16 +1405,16 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="H15" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1431,16 +1422,16 @@
         <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="G16" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1448,7 +1439,7 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1456,21 +1447,21 @@
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1481,7 +1472,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1490,7 +1481,7 @@
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1498,7 +1489,7 @@
         <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1511,16 +1502,16 @@
         <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1528,7 +1519,7 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
@@ -1538,32 +1529,32 @@
         <v>31</v>
       </c>
       <c r="F27" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
@@ -1575,12 +1566,12 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1588,7 +1579,7 @@
         <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -1596,7 +1587,7 @@
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1609,16 +1600,16 @@
         <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1626,7 +1617,7 @@
         <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -1634,32 +1625,32 @@
         <v>31</v>
       </c>
       <c r="F38" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F39" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -1669,12 +1660,12 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -1682,7 +1673,7 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -1695,16 +1686,16 @@
         <v>22</v>
       </c>
       <c r="E46" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -1712,16 +1703,16 @@
         <v>22</v>
       </c>
       <c r="E47" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F47" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -1731,7 +1722,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1739,7 +1730,7 @@
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1752,16 +1743,16 @@
         <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F52" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1769,7 +1760,7 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1777,27 +1768,27 @@
         <v>31</v>
       </c>
       <c r="F54" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F55" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1805,18 +1796,18 @@
         <v>60</v>
       </c>
       <c r="F56" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1826,7 +1817,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -1839,16 +1830,16 @@
         <v>22</v>
       </c>
       <c r="E61" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F61" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -1862,7 +1853,7 @@
         <v>51</v>
       </c>
       <c r="C63" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -1872,16 +1863,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F65" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -1899,16 +1890,16 @@
         <v>22</v>
       </c>
       <c r="E68" t="s">
-        <v>97</v>
+        <v>203</v>
       </c>
       <c r="F68" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -1921,7 +1912,7 @@
         <v>51</v>
       </c>
       <c r="C70" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -1931,30 +1922,30 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F72" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="F73" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -1964,13 +1955,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -1978,7 +1969,7 @@
         <v>51</v>
       </c>
       <c r="C77" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -1992,16 +1983,16 @@
         <v>22</v>
       </c>
       <c r="E79" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F79" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2009,7 +2000,7 @@
         <v>51</v>
       </c>
       <c r="C80" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2017,21 +2008,21 @@
         <v>22</v>
       </c>
       <c r="E81" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F81" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="H82" s="16"/>
     </row>
@@ -2050,16 +2041,16 @@
         <v>22</v>
       </c>
       <c r="E85" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F85" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -2070,7 +2061,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2087,13 +2078,13 @@
         <v>76</v>
       </c>
       <c r="F89" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="G89" t="s">
-        <v>95</v>
+        <v>209</v>
       </c>
       <c r="H89" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -2106,7 +2097,7 @@
         <v>51</v>
       </c>
       <c r="C91" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2116,21 +2107,21 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="G93" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="H93" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="E94" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -2141,7 +2132,7 @@
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
       <c r="B96" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2203,28 +2194,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="G2" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2232,31 +2223,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="I4" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2304,18 +2295,18 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>52</v>
@@ -2328,11 +2319,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,10 +2446,10 @@
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,13 +2457,13 @@
         <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>210</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2480,13 +2471,13 @@
         <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>212</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2494,191 +2485,193 @@
         <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" t="s">
         <v>89</v>
       </c>
+      <c r="B12" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"2"</f>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B14" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15" t="str">
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C15" t="s">
-        <v>113</v>
-      </c>
-      <c r="D15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" t="str">
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" t="str">
+      <c r="C17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18" t="str">
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" t="str">
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C21" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" t="s">
         <v>100</v>
       </c>
-      <c r="B20" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" t="str">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C21" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" t="str">
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,14 +2679,14 @@
         <v>56</v>
       </c>
       <c r="B24" t="str">
-        <f>"1"</f>
-        <v>1</v>
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2701,44 +2694,74 @@
         <v>56</v>
       </c>
       <c r="B25" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C25" t="s">
-        <v>157</v>
-      </c>
-      <c r="D25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="str">
+      <c r="C27" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C26" t="s">
-        <v>159</v>
-      </c>
-      <c r="D26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" t="str">
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C27" t="s">
-        <v>161</v>
-      </c>
-      <c r="D27" t="s">
-        <v>162</v>
+      <c r="C29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2751,7 +2774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
@@ -2776,7 +2799,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -2820,7 +2843,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -2831,7 +2854,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -2842,7 +2865,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -2853,7 +2876,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -2864,7 +2887,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -2875,7 +2898,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -2886,7 +2909,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
@@ -2897,7 +2920,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -2908,7 +2931,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -2919,7 +2942,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -2930,10 +2953,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -2941,7 +2964,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -2952,10 +2975,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -2963,10 +2986,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -2974,7 +2997,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -2985,7 +3008,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -2996,7 +3019,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -3007,7 +3030,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
         <v>60</v>
@@ -3018,10 +3041,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -3029,10 +3052,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -3040,10 +3063,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -3051,10 +3074,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Canges in questions if child dies
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA_VISIT/forms/CRIANCA_VISIT/CRIANCA_VISIT.xlsx
+++ b/app/config/tables/CRIANCA_VISIT/forms/CRIANCA_VISIT/CRIANCA_VISIT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B890BB1-4AC9-4D80-BE99-446135F29CA2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE0DBB-BA3E-440E-83E6-F59662FE093B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="285">
   <si>
     <t>setting_name</t>
   </si>
@@ -1566,11 +1566,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:M177"/>
+  <dimension ref="A1:M175"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C171" sqref="C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,20 +1812,20 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
       <c r="B21" t="s">
         <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
       <c r="B22" t="s">
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,35 +1918,47 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>279</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
       <c r="B32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" t="s">
-        <v>279</v>
+        <v>46</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s">
-        <v>181</v>
-      </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="A33" s="24"/>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" t="s">
+        <v>276</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>280</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -1954,64 +1966,50 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
       <c r="D35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" t="s">
-        <v>80</v>
+        <v>207</v>
       </c>
       <c r="F35" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>280</v>
-      </c>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
+      <c r="D36" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" t="s">
+        <v>278</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
-      <c r="D37" t="s">
-        <v>207</v>
-      </c>
-      <c r="F37" t="s">
-        <v>277</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>165</v>
-      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" t="s">
-        <v>278</v>
-      </c>
-      <c r="G38" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>213</v>
-      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
       <c r="B39" t="s">
         <v>91</v>
       </c>
@@ -2019,31 +2017,56 @@
       <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+      <c r="A40" s="12"/>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>91</v>
-      </c>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-    </row>
-    <row r="42" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>91</v>
-      </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
+      <c r="A41" s="12"/>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" t="s">
+        <v>81</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" t="s">
+        <v>84</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
+        <v>191</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
@@ -2054,119 +2077,106 @@
         <v>22</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="D45" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" t="s">
-        <v>83</v>
-      </c>
-      <c r="F45" t="s">
-        <v>84</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>86</v>
-      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" t="s">
-        <v>191</v>
+        <v>47</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" t="s">
-        <v>87</v>
-      </c>
-      <c r="F47" t="s">
-        <v>88</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="A47" s="25"/>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" t="s">
-        <v>91</v>
-      </c>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
+      <c r="A48" s="25"/>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" s="15" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" t="s">
+      <c r="A49" s="25"/>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>80</v>
+      </c>
+      <c r="F49" t="s">
+        <v>113</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="25"/>
+      <c r="B50" t="s">
         <v>47</v>
-      </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" t="s">
-        <v>181</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
       <c r="B51" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="C51" t="s">
+        <v>184</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="D52" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" t="s">
-        <v>80</v>
-      </c>
-      <c r="F52" t="s">
-        <v>114</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>115</v>
-      </c>
+      <c r="A52" s="26"/>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="D53" t="s">
         <v>22</v>
       </c>
@@ -2174,132 +2184,129 @@
         <v>80</v>
       </c>
       <c r="F53" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
+      <c r="A54" s="26"/>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C54" t="s">
+        <v>179</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>91</v>
-      </c>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
+      <c r="A55" s="26"/>
+      <c r="D55" t="s">
+        <v>207</v>
+      </c>
+      <c r="F55" t="s">
+        <v>166</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" t="s">
-        <v>184</v>
-      </c>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15"/>
+      <c r="A56" s="26"/>
+      <c r="D56" t="s">
+        <v>151</v>
+      </c>
+      <c r="F56" t="s">
+        <v>167</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H56" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="26"/>
-      <c r="B57" t="s">
-        <v>46</v>
-      </c>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F57" t="s">
+        <v>168</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="26"/>
-      <c r="D58" t="s">
-        <v>22</v>
-      </c>
-      <c r="E58" t="s">
-        <v>80</v>
-      </c>
-      <c r="F58" t="s">
-        <v>119</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>180</v>
-      </c>
+      <c r="B58" t="s">
+        <v>91</v>
+      </c>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" t="s">
-        <v>51</v>
-      </c>
-      <c r="C59" t="s">
-        <v>179</v>
+        <v>47</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
-      <c r="D60" t="s">
-        <v>207</v>
-      </c>
-      <c r="F60" t="s">
-        <v>166</v>
-      </c>
-      <c r="G60" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>169</v>
-      </c>
+      <c r="B60" t="s">
+        <v>91</v>
+      </c>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="D61" t="s">
-        <v>151</v>
-      </c>
-      <c r="F61" t="s">
-        <v>167</v>
-      </c>
-      <c r="G61" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>170</v>
-      </c>
+      <c r="B61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="26"/>
-      <c r="D62" t="s">
-        <v>58</v>
-      </c>
-      <c r="F62" t="s">
-        <v>168</v>
-      </c>
-      <c r="G62" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="H62" s="15" t="s">
-        <v>171</v>
-      </c>
+      <c r="A62" s="27"/>
+      <c r="B62" t="s">
+        <v>46</v>
+      </c>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
-      <c r="B63" t="s">
-        <v>91</v>
-      </c>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15"/>
+      <c r="A63" s="27"/>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63" t="s">
+        <v>118</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="H63" s="15" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="27"/>
       <c r="B64" t="s">
         <v>47</v>
       </c>
@@ -2308,13 +2315,16 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>91</v>
+        <v>51</v>
+      </c>
+      <c r="C65" t="s">
+        <v>209</v>
       </c>
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
+      <c r="A66" s="28"/>
       <c r="B66" t="s">
         <v>46</v>
       </c>
@@ -2322,137 +2332,138 @@
       <c r="H66" s="15"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
+      <c r="A67" s="28"/>
       <c r="D67" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" t="s">
-        <v>80</v>
-      </c>
-      <c r="F67" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>117</v>
+        <v>211</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>117</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
-      <c r="B68" t="s">
-        <v>47</v>
+      <c r="A68" s="28"/>
+      <c r="D68" t="s">
+        <v>156</v>
+      </c>
+      <c r="E68" t="s">
+        <v>210</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="28"/>
       <c r="B69" t="s">
-        <v>51</v>
-      </c>
-      <c r="C69" t="s">
-        <v>209</v>
+        <v>47</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="28"/>
       <c r="B70" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="15"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="28"/>
-      <c r="D71" t="s">
-        <v>153</v>
-      </c>
-      <c r="G71" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="H71" s="15" t="s">
-        <v>211</v>
-      </c>
+      <c r="A71" s="13"/>
+      <c r="B71" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" t="s">
+        <v>148</v>
+      </c>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="28"/>
-      <c r="D72" t="s">
-        <v>156</v>
-      </c>
-      <c r="E72" t="s">
-        <v>210</v>
+      <c r="A72" s="22"/>
+      <c r="B72" t="s">
+        <v>46</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="15"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="28"/>
-      <c r="B73" t="s">
+      <c r="A73" s="22"/>
+      <c r="D73" t="s">
+        <v>151</v>
+      </c>
+      <c r="F73" t="s">
+        <v>120</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="L73" t="s">
+        <v>275</v>
+      </c>
+      <c r="M73" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="22"/>
+      <c r="B74" t="s">
         <v>47</v>
-      </c>
-      <c r="G73" s="15"/>
-      <c r="H73" s="15"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>91</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="15"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C75" t="s">
-        <v>148</v>
+      <c r="A75" s="21"/>
+      <c r="B75" t="s">
+        <v>46</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="15"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
-      <c r="B76" t="s">
-        <v>46</v>
-      </c>
-      <c r="G76" s="15"/>
-      <c r="H76" s="15"/>
+      <c r="A76" s="21"/>
+      <c r="D76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" t="s">
+        <v>192</v>
+      </c>
+      <c r="F76" t="s">
+        <v>121</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="22"/>
-      <c r="D77" t="s">
-        <v>151</v>
-      </c>
-      <c r="F77" t="s">
-        <v>120</v>
-      </c>
-      <c r="G77" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="H77" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="L77" t="s">
-        <v>275</v>
-      </c>
-      <c r="M77" t="s">
-        <v>275</v>
-      </c>
+      <c r="A77" s="21"/>
+      <c r="B77" t="s">
+        <v>47</v>
+      </c>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
-      <c r="B78" t="s">
-        <v>47</v>
+      <c r="A78" s="14"/>
+      <c r="B78" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" t="s">
+        <v>131</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="15"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="21"/>
+      <c r="A79" s="20"/>
       <c r="B79" t="s">
         <v>46</v>
       </c>
@@ -2460,243 +2471,243 @@
       <c r="H79" s="15"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
+      <c r="A80" s="20"/>
       <c r="D80" t="s">
-        <v>22</v>
-      </c>
-      <c r="E80" t="s">
-        <v>192</v>
+        <v>151</v>
       </c>
       <c r="F80" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="21"/>
-      <c r="B81" t="s">
+      <c r="A81" s="20"/>
+      <c r="D81" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" t="s">
+        <v>123</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="20"/>
+      <c r="B82" t="s">
         <v>47</v>
-      </c>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C82" t="s">
-        <v>131</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="15"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
-      <c r="B83" t="s">
-        <v>46</v>
+      <c r="A83" s="14"/>
+      <c r="B83" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="15"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
-      <c r="D84" t="s">
-        <v>151</v>
-      </c>
-      <c r="F84" t="s">
-        <v>122</v>
-      </c>
-      <c r="G84" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="H84" s="15" t="s">
-        <v>132</v>
-      </c>
+      <c r="A84" s="12"/>
+      <c r="B84" t="s">
+        <v>46</v>
+      </c>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
+      <c r="A85" s="12"/>
       <c r="D85" t="s">
-        <v>151</v>
+        <v>22</v>
+      </c>
+      <c r="E85" t="s">
+        <v>80</v>
       </c>
       <c r="F85" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="20"/>
-      <c r="B86" t="s">
-        <v>47</v>
+      <c r="A86" s="10"/>
+      <c r="B86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" t="s">
+        <v>152</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="15"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
-      <c r="B87" s="14" t="s">
+      <c r="A87" s="12"/>
+      <c r="D87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" t="s">
+        <v>80</v>
+      </c>
+      <c r="F87" t="s">
+        <v>126</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H87" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="B88" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="G87" s="15"/>
-      <c r="H87" s="15"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="B88" t="s">
-        <v>46</v>
       </c>
       <c r="G88" s="15"/>
       <c r="H88" s="15"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
-      <c r="D89" t="s">
-        <v>22</v>
-      </c>
-      <c r="E89" t="s">
-        <v>80</v>
-      </c>
-      <c r="F89" t="s">
-        <v>124</v>
-      </c>
-      <c r="G89" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H89" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="B89" t="s">
+        <v>47</v>
+      </c>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C90" t="s">
-        <v>152</v>
+      <c r="A90" s="13"/>
+      <c r="B90" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="15"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
-      <c r="D91" t="s">
-        <v>22</v>
-      </c>
-      <c r="E91" t="s">
-        <v>80</v>
-      </c>
-      <c r="F91" t="s">
-        <v>126</v>
-      </c>
-      <c r="G91" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="H91" s="15" t="s">
-        <v>127</v>
-      </c>
+      <c r="B91" t="s">
+        <v>51</v>
+      </c>
+      <c r="C91" t="s">
+        <v>270</v>
+      </c>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-      <c r="B92" s="10" t="s">
-        <v>91</v>
+      <c r="A92" s="28"/>
+      <c r="B92" t="s">
+        <v>46</v>
       </c>
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" t="s">
-        <v>47</v>
-      </c>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
+      <c r="A93" s="28"/>
+      <c r="D93" t="s">
+        <v>153</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="H93" s="15" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
-      <c r="B94" s="13" t="s">
-        <v>91</v>
+      <c r="A94" s="28"/>
+      <c r="D94" t="s">
+        <v>156</v>
+      </c>
+      <c r="E94" t="s">
+        <v>215</v>
       </c>
       <c r="G94" s="15"/>
       <c r="H94" s="15"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="28"/>
       <c r="B95" t="s">
-        <v>51</v>
-      </c>
-      <c r="C95" t="s">
-        <v>270</v>
+        <v>47</v>
       </c>
       <c r="G95" s="15"/>
       <c r="H95" s="15"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="28"/>
       <c r="B96" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G96" s="15"/>
       <c r="H96" s="15"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="28"/>
-      <c r="D97" t="s">
-        <v>153</v>
-      </c>
-      <c r="G97" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>217</v>
-      </c>
+      <c r="B97" t="s">
+        <v>51</v>
+      </c>
+      <c r="C97" t="s">
+        <v>283</v>
+      </c>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="28"/>
-      <c r="D98" t="s">
-        <v>156</v>
-      </c>
-      <c r="E98" t="s">
-        <v>215</v>
+      <c r="A98" s="22"/>
+      <c r="B98" t="s">
+        <v>46</v>
       </c>
       <c r="G98" s="15"/>
       <c r="H98" s="15"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="28"/>
-      <c r="B99" t="s">
+      <c r="A99" s="22"/>
+      <c r="D99" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99" t="s">
+        <v>80</v>
+      </c>
+      <c r="F99" t="s">
+        <v>219</v>
+      </c>
+      <c r="G99" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="H99" s="15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="22"/>
+      <c r="B100" t="s">
         <v>47</v>
-      </c>
-      <c r="G99" s="15"/>
-      <c r="H99" s="15"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>91</v>
       </c>
       <c r="G100" s="15"/>
       <c r="H100" s="15"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
+      <c r="A101" s="29"/>
+      <c r="B101" s="29" t="s">
         <v>51</v>
       </c>
       <c r="C101" t="s">
-        <v>283</v>
+        <v>231</v>
       </c>
       <c r="G101" s="15"/>
       <c r="H101" s="15"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="22"/>
+      <c r="A102" s="6"/>
       <c r="B102" t="s">
         <v>46</v>
       </c>
@@ -2704,25 +2715,25 @@
       <c r="H102" s="15"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="22"/>
+      <c r="A103" s="6"/>
       <c r="D103" t="s">
-        <v>22</v>
+        <v>220</v>
       </c>
       <c r="E103" t="s">
-        <v>80</v>
+        <v>222</v>
       </c>
       <c r="F103" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G103" s="15" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H103" s="15" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="22"/>
+      <c r="A104" s="6"/>
       <c r="B104" t="s">
         <v>47</v>
       </c>
@@ -2730,277 +2741,274 @@
       <c r="H104" s="15"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
-      <c r="B105" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C105" t="s">
-        <v>231</v>
+      <c r="A105" s="30"/>
+      <c r="B105" t="s">
+        <v>46</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="15"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="6"/>
-      <c r="B106" t="s">
-        <v>46</v>
-      </c>
-      <c r="G106" s="15"/>
-      <c r="H106" s="15"/>
+      <c r="A106" s="30"/>
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
+        <v>80</v>
+      </c>
+      <c r="F106" t="s">
+        <v>228</v>
+      </c>
+      <c r="G106" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="H106" s="15" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="6"/>
-      <c r="D107" t="s">
-        <v>220</v>
-      </c>
-      <c r="E107" t="s">
-        <v>222</v>
-      </c>
-      <c r="F107" t="s">
-        <v>221</v>
-      </c>
-      <c r="G107" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="H107" s="15" t="s">
-        <v>222</v>
-      </c>
+      <c r="A107" s="30"/>
+      <c r="B107" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C107" t="s">
+        <v>230</v>
+      </c>
+      <c r="G107" s="15"/>
+      <c r="H107" s="15"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="6"/>
-      <c r="B108" t="s">
-        <v>47</v>
-      </c>
-      <c r="G108" s="15"/>
-      <c r="H108" s="15"/>
+      <c r="A108" s="30"/>
+      <c r="D108" t="s">
+        <v>207</v>
+      </c>
+      <c r="F108" t="s">
+        <v>232</v>
+      </c>
+      <c r="G108" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="H108" s="15" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="30"/>
-      <c r="B109" t="s">
-        <v>46</v>
-      </c>
-      <c r="G109" s="15"/>
-      <c r="H109" s="15"/>
+      <c r="D109" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" t="s">
+        <v>80</v>
+      </c>
+      <c r="F109" t="s">
+        <v>235</v>
+      </c>
+      <c r="G109" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="H109" s="15" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="30"/>
-      <c r="D110" t="s">
-        <v>22</v>
-      </c>
-      <c r="E110" t="s">
-        <v>80</v>
-      </c>
-      <c r="F110" t="s">
-        <v>228</v>
-      </c>
-      <c r="G110" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="H110" s="15" t="s">
-        <v>229</v>
-      </c>
+      <c r="B110" t="s">
+        <v>91</v>
+      </c>
+      <c r="G110" s="15"/>
+      <c r="H110" s="15"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="30"/>
-      <c r="B111" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C111" t="s">
-        <v>230</v>
+      <c r="B111" t="s">
+        <v>47</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111" s="15"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
-      <c r="D112" t="s">
-        <v>207</v>
-      </c>
-      <c r="F112" t="s">
-        <v>232</v>
-      </c>
-      <c r="G112" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="H112" s="15" t="s">
-        <v>233</v>
-      </c>
+      <c r="A112" s="19"/>
+      <c r="B112" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C112" t="s">
+        <v>230</v>
+      </c>
+      <c r="G112" s="15"/>
+      <c r="H112" s="15"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="30"/>
-      <c r="D113" t="s">
-        <v>22</v>
-      </c>
-      <c r="E113" t="s">
-        <v>80</v>
-      </c>
-      <c r="F113" t="s">
-        <v>235</v>
-      </c>
-      <c r="G113" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="H113" s="15" t="s">
-        <v>234</v>
-      </c>
+      <c r="A113" s="31"/>
+      <c r="B113" t="s">
+        <v>46</v>
+      </c>
+      <c r="G113" s="15"/>
+      <c r="H113" s="15"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
-      <c r="B114" t="s">
-        <v>91</v>
-      </c>
-      <c r="G114" s="15"/>
-      <c r="H114" s="15"/>
+      <c r="A114" s="31"/>
+      <c r="D114" t="s">
+        <v>22</v>
+      </c>
+      <c r="E114" t="s">
+        <v>239</v>
+      </c>
+      <c r="F114" t="s">
+        <v>237</v>
+      </c>
+      <c r="G114" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="H114" s="15" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
+      <c r="A115" s="31"/>
       <c r="B115" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C115" t="s">
+        <v>240</v>
       </c>
       <c r="G115" s="15"/>
       <c r="H115" s="15"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="19"/>
-      <c r="B116" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C116" t="s">
-        <v>230</v>
-      </c>
-      <c r="G116" s="15"/>
-      <c r="H116" s="15"/>
+      <c r="A116" s="31"/>
+      <c r="D116" t="s">
+        <v>58</v>
+      </c>
+      <c r="F116" t="s">
+        <v>242</v>
+      </c>
+      <c r="G116" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="H116" s="15" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="31"/>
       <c r="B117" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="15"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="31"/>
-      <c r="D118" t="s">
-        <v>22</v>
-      </c>
-      <c r="E118" t="s">
-        <v>239</v>
-      </c>
-      <c r="F118" t="s">
-        <v>237</v>
-      </c>
-      <c r="G118" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="H118" s="15" t="s">
-        <v>236</v>
-      </c>
+      <c r="B118" t="s">
+        <v>47</v>
+      </c>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="31"/>
+      <c r="A119" s="32"/>
       <c r="B119" t="s">
-        <v>51</v>
-      </c>
-      <c r="C119" t="s">
-        <v>240</v>
+        <v>46</v>
       </c>
       <c r="G119" s="15"/>
       <c r="H119" s="15"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="31"/>
+      <c r="A120" s="32"/>
       <c r="D120" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="E120" t="s">
+        <v>80</v>
       </c>
       <c r="F120" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G120" s="15" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="H120" s="15" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="31"/>
+      <c r="A121" s="32"/>
       <c r="B121" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="G121" s="15"/>
       <c r="H121" s="15"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="31"/>
+      <c r="A122" s="33"/>
       <c r="B122" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G122" s="15"/>
       <c r="H122" s="15"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="32"/>
-      <c r="B123" t="s">
-        <v>46</v>
-      </c>
-      <c r="G123" s="15"/>
-      <c r="H123" s="15"/>
+      <c r="A123" s="33"/>
+      <c r="D123" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" t="s">
+        <v>80</v>
+      </c>
+      <c r="F123" t="s">
+        <v>245</v>
+      </c>
+      <c r="G123" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H123" s="15" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="32"/>
-      <c r="D124" t="s">
-        <v>22</v>
-      </c>
-      <c r="E124" t="s">
-        <v>80</v>
-      </c>
-      <c r="F124" t="s">
-        <v>244</v>
-      </c>
-      <c r="G124" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="H124" s="15" t="s">
-        <v>243</v>
-      </c>
+      <c r="A124" s="33"/>
+      <c r="B124" t="s">
+        <v>51</v>
+      </c>
+      <c r="C124" t="s">
+        <v>249</v>
+      </c>
+      <c r="G124" s="15"/>
+      <c r="H124" s="15"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="32"/>
-      <c r="B125" t="s">
-        <v>47</v>
-      </c>
-      <c r="G125" s="15"/>
-      <c r="H125" s="15"/>
+      <c r="A125" s="33"/>
+      <c r="D125" t="s">
+        <v>58</v>
+      </c>
+      <c r="F125" t="s">
+        <v>247</v>
+      </c>
+      <c r="G125" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="H125" s="15" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="33"/>
       <c r="B126" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G126" s="15"/>
       <c r="H126" s="15"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="33"/>
-      <c r="D127" t="s">
-        <v>22</v>
-      </c>
-      <c r="E127" t="s">
-        <v>80</v>
-      </c>
-      <c r="F127" t="s">
-        <v>245</v>
-      </c>
-      <c r="G127" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="H127" s="15" t="s">
-        <v>246</v>
-      </c>
+      <c r="B127" t="s">
+        <v>47</v>
+      </c>
+      <c r="G127" s="15"/>
+      <c r="H127" s="15"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="33"/>
+      <c r="A128" s="34"/>
       <c r="B128" t="s">
         <v>51</v>
       </c>
@@ -3011,350 +3019,350 @@
       <c r="H128" s="15"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="33"/>
-      <c r="D129" t="s">
-        <v>58</v>
-      </c>
-      <c r="F129" t="s">
-        <v>247</v>
-      </c>
-      <c r="G129" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="H129" s="15" t="s">
-        <v>248</v>
-      </c>
+      <c r="A129" s="34"/>
+      <c r="B129" t="s">
+        <v>46</v>
+      </c>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="33"/>
-      <c r="B130" t="s">
-        <v>91</v>
-      </c>
-      <c r="G130" s="15"/>
-      <c r="H130" s="15"/>
+      <c r="A130" s="34"/>
+      <c r="D130" t="s">
+        <v>22</v>
+      </c>
+      <c r="E130" t="s">
+        <v>80</v>
+      </c>
+      <c r="F130" t="s">
+        <v>250</v>
+      </c>
+      <c r="G130" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="H130" s="15" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="33"/>
+      <c r="A131" s="34"/>
       <c r="B131" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C131" t="s">
+        <v>254</v>
       </c>
       <c r="G131" s="15"/>
       <c r="H131" s="15"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="34"/>
-      <c r="B132" t="s">
-        <v>51</v>
-      </c>
-      <c r="C132" t="s">
-        <v>249</v>
-      </c>
-      <c r="G132" s="15"/>
-      <c r="H132" s="15"/>
+      <c r="D132" t="s">
+        <v>58</v>
+      </c>
+      <c r="F132" t="s">
+        <v>252</v>
+      </c>
+      <c r="G132" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="H132" s="15" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="34"/>
       <c r="B133" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G133" s="15"/>
       <c r="H133" s="15"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="34"/>
-      <c r="D134" t="s">
-        <v>22</v>
-      </c>
-      <c r="E134" t="s">
-        <v>80</v>
-      </c>
-      <c r="F134" t="s">
-        <v>250</v>
-      </c>
-      <c r="G134" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="H134" s="15" t="s">
-        <v>251</v>
-      </c>
+      <c r="B134" t="s">
+        <v>47</v>
+      </c>
+      <c r="G134" s="15"/>
+      <c r="H134" s="15"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="34"/>
       <c r="B135" t="s">
-        <v>51</v>
-      </c>
-      <c r="C135" t="s">
-        <v>254</v>
+        <v>91</v>
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="15"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" s="34"/>
-      <c r="D136" t="s">
-        <v>58</v>
-      </c>
-      <c r="F136" t="s">
-        <v>252</v>
-      </c>
-      <c r="G136" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="H136" s="15" t="s">
-        <v>253</v>
-      </c>
+      <c r="A136" s="25"/>
+      <c r="B136" t="s">
+        <v>46</v>
+      </c>
+      <c r="G136" s="15"/>
+      <c r="H136" s="15"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
-      <c r="B137" t="s">
-        <v>91</v>
-      </c>
-      <c r="G137" s="15"/>
-      <c r="H137" s="15"/>
+      <c r="A137" s="25"/>
+      <c r="D137" t="s">
+        <v>22</v>
+      </c>
+      <c r="E137" t="s">
+        <v>80</v>
+      </c>
+      <c r="F137" t="s">
+        <v>255</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="H137" s="15" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
+      <c r="A138" s="25"/>
       <c r="B138" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C138" t="s">
+        <v>258</v>
       </c>
       <c r="G138" s="15"/>
       <c r="H138" s="15"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="34"/>
-      <c r="B139" t="s">
-        <v>91</v>
-      </c>
-      <c r="G139" s="15"/>
-      <c r="H139" s="15"/>
+      <c r="A139" s="25"/>
+      <c r="D139" t="s">
+        <v>207</v>
+      </c>
+      <c r="F139" t="s">
+        <v>257</v>
+      </c>
+      <c r="G139" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="H139" s="15" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="25"/>
-      <c r="B140" t="s">
-        <v>46</v>
-      </c>
-      <c r="G140" s="15"/>
-      <c r="H140" s="15"/>
+      <c r="D140" t="s">
+        <v>22</v>
+      </c>
+      <c r="E140" t="s">
+        <v>80</v>
+      </c>
+      <c r="F140" t="s">
+        <v>271</v>
+      </c>
+      <c r="G140" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="H140" s="15" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="25"/>
-      <c r="D141" t="s">
-        <v>22</v>
-      </c>
-      <c r="E141" t="s">
-        <v>80</v>
-      </c>
-      <c r="F141" t="s">
-        <v>255</v>
-      </c>
-      <c r="G141" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="H141" s="15" t="s">
-        <v>256</v>
-      </c>
+      <c r="B141" t="s">
+        <v>91</v>
+      </c>
+      <c r="G141" s="15"/>
+      <c r="H141" s="15"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="25"/>
       <c r="B142" t="s">
-        <v>51</v>
-      </c>
-      <c r="C142" t="s">
-        <v>258</v>
+        <v>47</v>
       </c>
       <c r="G142" s="15"/>
       <c r="H142" s="15"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="25"/>
-      <c r="D143" t="s">
-        <v>207</v>
-      </c>
-      <c r="F143" t="s">
-        <v>257</v>
-      </c>
-      <c r="G143" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="H143" s="15" t="s">
-        <v>233</v>
-      </c>
+      <c r="A143" s="35"/>
+      <c r="B143" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C143" t="s">
+        <v>259</v>
+      </c>
+      <c r="G143" s="15"/>
+      <c r="H143" s="15"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="25"/>
-      <c r="D144" t="s">
-        <v>22</v>
-      </c>
-      <c r="E144" t="s">
-        <v>80</v>
-      </c>
-      <c r="F144" t="s">
-        <v>271</v>
-      </c>
-      <c r="G144" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="H144" s="15" t="s">
-        <v>234</v>
-      </c>
+      <c r="A144" s="26"/>
+      <c r="B144" t="s">
+        <v>46</v>
+      </c>
+      <c r="G144" s="15"/>
+      <c r="H144" s="15"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A145" s="25"/>
-      <c r="B145" t="s">
-        <v>91</v>
-      </c>
-      <c r="G145" s="15"/>
-      <c r="H145" s="15"/>
+      <c r="A145" s="26"/>
+      <c r="D145" t="s">
+        <v>22</v>
+      </c>
+      <c r="E145" t="s">
+        <v>239</v>
+      </c>
+      <c r="F145" t="s">
+        <v>260</v>
+      </c>
+      <c r="G145" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="H145" s="15" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A146" s="25"/>
+      <c r="A146" s="26"/>
       <c r="B146" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C146" t="s">
+        <v>269</v>
       </c>
       <c r="G146" s="15"/>
       <c r="H146" s="15"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A147" s="35"/>
-      <c r="B147" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C147" t="s">
-        <v>259</v>
-      </c>
-      <c r="G147" s="15"/>
-      <c r="H147" s="15"/>
+      <c r="A147" s="26"/>
+      <c r="D147" t="s">
+        <v>58</v>
+      </c>
+      <c r="F147" t="s">
+        <v>261</v>
+      </c>
+      <c r="G147" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="H147" s="15" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="26"/>
       <c r="B148" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G148" s="15"/>
       <c r="H148" s="15"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="26"/>
-      <c r="D149" t="s">
-        <v>22</v>
-      </c>
-      <c r="E149" t="s">
-        <v>239</v>
-      </c>
-      <c r="F149" t="s">
-        <v>260</v>
-      </c>
-      <c r="G149" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="H149" s="15" t="s">
-        <v>236</v>
-      </c>
+      <c r="B149" t="s">
+        <v>47</v>
+      </c>
+      <c r="G149" s="15"/>
+      <c r="H149" s="15"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="26"/>
+      <c r="A150" s="36"/>
       <c r="B150" t="s">
-        <v>51</v>
-      </c>
-      <c r="C150" t="s">
-        <v>269</v>
+        <v>46</v>
       </c>
       <c r="G150" s="15"/>
       <c r="H150" s="15"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A151" s="26"/>
+      <c r="A151" s="36"/>
       <c r="D151" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="E151" t="s">
+        <v>80</v>
       </c>
       <c r="F151" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G151" s="15" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="H151" s="15" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A152" s="26"/>
+      <c r="A152" s="36"/>
       <c r="B152" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="G152" s="15"/>
       <c r="H152" s="15"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A153" s="26"/>
+      <c r="A153" s="27"/>
       <c r="B153" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G153" s="15"/>
       <c r="H153" s="15"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A154" s="36"/>
-      <c r="B154" t="s">
-        <v>46</v>
-      </c>
-      <c r="G154" s="15"/>
-      <c r="H154" s="15"/>
+      <c r="A154" s="27"/>
+      <c r="D154" t="s">
+        <v>22</v>
+      </c>
+      <c r="E154" t="s">
+        <v>80</v>
+      </c>
+      <c r="F154" t="s">
+        <v>263</v>
+      </c>
+      <c r="G154" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H154" s="15" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" s="36"/>
-      <c r="D155" t="s">
-        <v>22</v>
-      </c>
-      <c r="E155" t="s">
-        <v>80</v>
-      </c>
-      <c r="F155" t="s">
-        <v>262</v>
-      </c>
-      <c r="G155" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="H155" s="15" t="s">
-        <v>243</v>
-      </c>
+      <c r="A155" s="27"/>
+      <c r="B155" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155" t="s">
+        <v>268</v>
+      </c>
+      <c r="G155" s="15"/>
+      <c r="H155" s="15"/>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="36"/>
-      <c r="B156" t="s">
-        <v>47</v>
-      </c>
-      <c r="G156" s="15"/>
-      <c r="H156" s="15"/>
+      <c r="A156" s="27"/>
+      <c r="D156" t="s">
+        <v>58</v>
+      </c>
+      <c r="F156" t="s">
+        <v>264</v>
+      </c>
+      <c r="G156" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="H156" s="15" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="27"/>
       <c r="B157" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G157" s="15"/>
       <c r="H157" s="15"/>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="27"/>
-      <c r="D158" t="s">
-        <v>22</v>
-      </c>
-      <c r="E158" t="s">
-        <v>80</v>
-      </c>
-      <c r="F158" t="s">
-        <v>263</v>
-      </c>
-      <c r="G158" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="H158" s="15" t="s">
-        <v>246</v>
-      </c>
+      <c r="B158" t="s">
+        <v>47</v>
+      </c>
+      <c r="G158" s="15"/>
+      <c r="H158" s="15"/>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A159" s="27"/>
+      <c r="A159" s="28"/>
       <c r="B159" t="s">
         <v>51</v>
       </c>
@@ -3365,179 +3373,151 @@
       <c r="H159" s="15"/>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A160" s="27"/>
-      <c r="D160" t="s">
-        <v>58</v>
-      </c>
-      <c r="F160" t="s">
-        <v>264</v>
-      </c>
-      <c r="G160" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="H160" s="15" t="s">
-        <v>248</v>
-      </c>
+      <c r="A160" s="28"/>
+      <c r="B160" t="s">
+        <v>46</v>
+      </c>
+      <c r="G160" s="15"/>
+      <c r="H160" s="15"/>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A161" s="27"/>
-      <c r="B161" t="s">
-        <v>91</v>
-      </c>
-      <c r="G161" s="15"/>
-      <c r="H161" s="15"/>
+      <c r="A161" s="28"/>
+      <c r="D161" t="s">
+        <v>22</v>
+      </c>
+      <c r="E161" t="s">
+        <v>80</v>
+      </c>
+      <c r="F161" t="s">
+        <v>265</v>
+      </c>
+      <c r="G161" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="H161" s="15" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A162" s="27"/>
+      <c r="A162" s="28"/>
       <c r="B162" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C162" t="s">
+        <v>267</v>
       </c>
       <c r="G162" s="15"/>
       <c r="H162" s="15"/>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="28"/>
-      <c r="B163" t="s">
-        <v>51</v>
-      </c>
-      <c r="C163" t="s">
-        <v>268</v>
-      </c>
-      <c r="G163" s="15"/>
-      <c r="H163" s="15"/>
+      <c r="D163" t="s">
+        <v>58</v>
+      </c>
+      <c r="F163" t="s">
+        <v>266</v>
+      </c>
+      <c r="G163" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="H163" s="15" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="28"/>
       <c r="B164" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G164" s="15"/>
       <c r="H164" s="15"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="28"/>
-      <c r="D165" t="s">
-        <v>22</v>
-      </c>
-      <c r="E165" t="s">
-        <v>80</v>
-      </c>
-      <c r="F165" t="s">
-        <v>265</v>
-      </c>
-      <c r="G165" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="H165" s="15" t="s">
-        <v>251</v>
-      </c>
+      <c r="B165" t="s">
+        <v>47</v>
+      </c>
+      <c r="G165" s="15"/>
+      <c r="H165" s="15"/>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="28"/>
       <c r="B166" t="s">
-        <v>51</v>
-      </c>
-      <c r="C166" t="s">
-        <v>267</v>
+        <v>91</v>
       </c>
       <c r="G166" s="15"/>
       <c r="H166" s="15"/>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A167" s="28"/>
-      <c r="D167" t="s">
-        <v>58</v>
-      </c>
-      <c r="F167" t="s">
-        <v>266</v>
-      </c>
-      <c r="G167" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="H167" s="15" t="s">
-        <v>253</v>
-      </c>
+      <c r="A167" s="33"/>
+      <c r="B167" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="G167" s="15"/>
+      <c r="H167" s="15"/>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A168" s="28"/>
-      <c r="B168" t="s">
+      <c r="A168" s="19"/>
+      <c r="B168" s="19" t="s">
         <v>91</v>
       </c>
       <c r="G168" s="15"/>
       <c r="H168" s="15"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" s="28"/>
-      <c r="B169" t="s">
+      <c r="A169" s="29"/>
+      <c r="B169" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="15"/>
+      <c r="B170" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="15"/>
+      <c r="B171" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="21"/>
+      <c r="B172" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="21"/>
+      <c r="D173" t="s">
+        <v>22</v>
+      </c>
+      <c r="E173" t="s">
+        <v>80</v>
+      </c>
+      <c r="F173" t="s">
+        <v>128</v>
+      </c>
+      <c r="G173" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H173" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="21"/>
+      <c r="B174" t="s">
         <v>47</v>
       </c>
-      <c r="G169" s="15"/>
-      <c r="H169" s="15"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" s="28"/>
-      <c r="B170" t="s">
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
         <v>91</v>
-      </c>
-      <c r="G170" s="15"/>
-      <c r="H170" s="15"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A171" s="33"/>
-      <c r="B171" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="G171" s="15"/>
-      <c r="H171" s="15"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A172" s="19"/>
-      <c r="B172" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="G172" s="15"/>
-      <c r="H172" s="15"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A173" s="29"/>
-      <c r="B173" s="29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="15"/>
-      <c r="B174" s="15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" s="21"/>
-      <c r="B175" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A176" s="21"/>
-      <c r="D176" t="s">
-        <v>22</v>
-      </c>
-      <c r="E176" t="s">
-        <v>80</v>
-      </c>
-      <c r="F176" t="s">
-        <v>128</v>
-      </c>
-      <c r="G176" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H176" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="21"/>
-      <c r="B177" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -4346,7 +4326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>

</xml_diff>